<commit_message>
Added 3 threads in main method
</commit_message>
<xml_diff>
--- a/Labs/Lab 9/city_locations_test.xlsx
+++ b/Labs/Lab 9/city_locations_test.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Google Drive\BCIT Work Synced Folder\My Courses\COMP3522 OOP 2\Fall 2019\Week 12\Lecture 1\W12 L1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eric\PycharmProjects\3522_A01037479\Labs\Lab 9\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5C6025A-63D0-487C-B1B6-13C5A0E9ADA2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E286633-E9C3-4A64-8271-384AFB73F5D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25095" yWindow="2280" windowWidth="22815" windowHeight="14850" xr2:uid="{86E8A028-58B2-4029-8ACE-F76B7C3B81F8}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{86E8A028-58B2-4029-8ACE-F76B7C3B81F8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -415,17 +415,17 @@
   <dimension ref="A1:C158"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C8" sqref="A7:C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.28515625" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" customWidth="1"/>
-    <col min="3" max="3" width="15.140625" customWidth="1"/>
+    <col min="1" max="1" width="19.26953125" customWidth="1"/>
+    <col min="2" max="2" width="11.453125" customWidth="1"/>
+    <col min="3" max="3" width="15.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -436,7 +436,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -447,7 +447,7 @@
         <v>-123.1216</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -458,7 +458,7 @@
         <v>-114.39700000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -469,7 +469,7 @@
         <v>-112.81659999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -480,7 +480,7 @@
         <v>-125.25</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -491,7 +491,7 @@
         <v>-118.1833</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -502,7 +502,7 @@
         <v>-108.43470000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -513,7 +513,7 @@
         <v>-73.583299999999994</v>
       </c>
     </row>
-    <row r="158" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="158" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>